<commit_message>
Ke hoach lam viec
</commit_message>
<xml_diff>
--- a/Documents/Kế hoạch làm việc.xlsx
+++ b/Documents/Kế hoạch làm việc.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17030"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_CE56DC7EAB1752B6F509CA20F681052C332C3AEC" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{D14F90CE-747B-494C-A7F6-3EDE69CD35E9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -97,12 +98,15 @@
   </si>
   <si>
     <t>Hoàng</t>
+  </si>
+  <si>
+    <t>Thành</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -301,13 +305,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -334,6 +337,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -343,10 +361,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
@@ -357,21 +375,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -686,116 +689,116 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="24.375" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="18" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="20" t="s">
+      <c r="E2" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="20"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="20" t="s">
+      <c r="F2" s="24"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="20"/>
+      <c r="J2" s="24"/>
     </row>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22"/>
+      <c r="C3" s="26"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="21" t="s">
+      <c r="E3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="22"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22"/>
+      <c r="F3" s="26"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="26"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="22"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="21" t="s">
+      <c r="E4" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="22"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="22"/>
+      <c r="F4" s="26"/>
+      <c r="H4" s="9"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="26"/>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="23" t="s">
+      <c r="B5" s="22"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="24"/>
+      <c r="F5" s="23"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="23"/>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="23" t="s">
+      <c r="C6" s="23"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="24"/>
-      <c r="H6" s="12"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="24"/>
+      <c r="F6" s="23"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="23"/>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" s="16"/>
-      <c r="I7" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="32" t="s">
+      <c r="D7" s="13"/>
+      <c r="E7" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="15"/>
+      <c r="I7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J7" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="26"/>
-      <c r="C8" s="25" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -807,85 +810,85 @@
       <c r="F8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I8" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="32" t="s">
+      <c r="I8" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J8" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="5" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="11" t="s">
+      <c r="F9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I9" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J9" s="32" t="s">
+      <c r="I9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J9" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H10" s="11" t="s">
+      <c r="F10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I10" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="32" t="s">
+      <c r="I10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B11" s="26"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="8" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="31"/>
+      <c r="D11" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H11" s="12" t="s">
+      <c r="E11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J11" s="32" t="s">
+      <c r="I11" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J11" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B12" s="26"/>
-      <c r="C12" s="25" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="29" t="s">
         <v>18</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -897,270 +900,288 @@
       <c r="F12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J12" s="32" t="s">
+      <c r="I12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="5" t="s">
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" t="s">
         <v>20</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="11" t="s">
+      <c r="F13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J13" s="32" t="s">
+      <c r="I13" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J13" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="5" t="s">
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="11" t="s">
+      <c r="F14" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H14" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J14" s="32" t="s">
+      <c r="I14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J14" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="26"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="8" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H15" s="12" t="s">
+      <c r="E15" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="32" t="s">
+      <c r="I15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J15" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="26"/>
-      <c r="C16" s="25" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" t="s">
         <v>19</v>
       </c>
       <c r="E16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H16" s="11" t="s">
+      <c r="F16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H16" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="32" t="s">
+      <c r="I16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J16" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="5" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" t="s">
         <v>20</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H17" s="11" t="s">
+      <c r="F17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J17" s="32" t="s">
+      <c r="I17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J17" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="5" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="H18" s="11" t="s">
+      <c r="F18" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="J18" s="32" t="s">
+      <c r="I18" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J18" s="19" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="8" t="s">
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E19" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H19" s="12" t="s">
+      <c r="E19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="I19" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J19" s="19" t="s">
+      <c r="I19" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="J19" s="18" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="29"/>
-      <c r="D20" s="14"/>
-      <c r="E20" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="16"/>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="16"/>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" s="16"/>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
-      <c r="J23" s="17"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" s="16"/>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="17"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J24" s="16"/>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="H25" s="16"/>
-      <c r="I25" s="16"/>
-      <c r="J25" s="17"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1175,16 +1196,6 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="B21:C21"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Long vua thay doi
</commit_message>
<xml_diff>
--- a/Documents/Kế hoạch làm việc.xlsx
+++ b/Documents/Kế hoạch làm việc.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E7D75AA-4174-4D1B-B0B9-39A7A3FD6541}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{365FB099-7F90-4EF3-9ACC-D2F91B4B14C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Model -Database</t>
+  </si>
+  <si>
+    <t>Long</t>
   </si>
 </sst>
 </file>
@@ -346,25 +349,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -698,97 +701,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6:J6"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B2" s="24" t="s">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="24"/>
+      <c r="C2" s="20"/>
       <c r="D2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="20"/>
       <c r="H2" s="15"/>
-      <c r="I2" s="24" t="s">
+      <c r="I2" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="24"/>
-    </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B3" s="25" t="s">
+      <c r="J2" s="20"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="26"/>
+      <c r="C3" s="22"/>
       <c r="D3" s="2"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="26"/>
+      <c r="F3" s="22"/>
       <c r="H3" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="25" t="s">
+      <c r="I3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="26"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B4" s="25" t="s">
+      <c r="J3" s="22"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="26"/>
+      <c r="C4" s="22"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="25" t="s">
+      <c r="E4" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="26"/>
+      <c r="F4" s="22"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="26"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B5" s="22"/>
-      <c r="C5" s="23"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="23"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="23"/>
+      <c r="F5" s="24"/>
       <c r="H5" s="11"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B6" s="22" t="s">
+      <c r="I5" s="23"/>
+      <c r="J5" s="24"/>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="23"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="F6" s="23"/>
+      <c r="F6" s="24"/>
       <c r="H6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="J6" s="23"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" s="29" t="s">
         <v>14</v>
       </c>
@@ -810,7 +813,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" s="30"/>
       <c r="C8" s="29" t="s">
         <v>18</v>
@@ -834,7 +837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" s="30"/>
       <c r="C9" s="30"/>
       <c r="D9" t="s">
@@ -856,7 +859,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="30"/>
       <c r="C10" s="30"/>
       <c r="D10" t="s">
@@ -878,7 +881,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" s="30"/>
       <c r="C11" s="31"/>
       <c r="D11" s="7" t="s">
@@ -900,7 +903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B12" s="30"/>
       <c r="C12" s="29" t="s">
         <v>18</v>
@@ -924,7 +927,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B13" s="30"/>
       <c r="C13" s="30"/>
       <c r="D13" t="s">
@@ -946,7 +949,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B14" s="30"/>
       <c r="C14" s="30"/>
       <c r="D14" t="s">
@@ -968,7 +971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B15" s="30"/>
       <c r="C15" s="31"/>
       <c r="D15" s="7" t="s">
@@ -990,7 +993,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="30"/>
       <c r="C16" s="29" t="s">
         <v>18</v>
@@ -1014,7 +1017,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="30"/>
       <c r="C17" s="30"/>
       <c r="D17" t="s">
@@ -1036,7 +1039,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B18" s="30"/>
       <c r="C18" s="30"/>
       <c r="D18" t="s">
@@ -1058,7 +1061,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B19" s="31"/>
       <c r="C19" s="31"/>
       <c r="D19" s="7" t="s">
@@ -1080,7 +1083,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B20" s="27" t="s">
         <v>5</v>
       </c>
@@ -1093,10 +1096,12 @@
         <v>17</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="15"/>
+      <c r="I20" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="J20" s="16"/>
     </row>
-    <row r="21" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B21" s="27" t="s">
         <v>6</v>
       </c>
@@ -1109,14 +1114,16 @@
         <v>17</v>
       </c>
       <c r="H21" s="15"/>
-      <c r="I21" s="15"/>
+      <c r="I21" s="15" t="s">
+        <v>29</v>
+      </c>
       <c r="J21" s="16"/>
     </row>
-    <row r="22" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B22" s="20" t="s">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B22" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="21"/>
+      <c r="C22" s="26"/>
       <c r="D22" s="17"/>
       <c r="E22" s="17" t="s">
         <v>16</v>
@@ -1128,11 +1135,11 @@
       <c r="I22" s="15"/>
       <c r="J22" s="16"/>
     </row>
-    <row r="23" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B23" s="20" t="s">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="21"/>
+      <c r="C23" s="26"/>
       <c r="D23" s="17"/>
       <c r="E23" s="17" t="s">
         <v>16</v>
@@ -1144,11 +1151,11 @@
       <c r="I23" s="15"/>
       <c r="J23" s="16"/>
     </row>
-    <row r="24" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B24" s="20" t="s">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C24" s="21"/>
+      <c r="C24" s="26"/>
       <c r="D24" s="17"/>
       <c r="E24" s="17" t="s">
         <v>16</v>
@@ -1160,11 +1167,11 @@
       <c r="I24" s="15"/>
       <c r="J24" s="16"/>
     </row>
-    <row r="25" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="B25" s="22" t="s">
+    <row r="25" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B25" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="23"/>
+      <c r="C25" s="24"/>
       <c r="D25" s="17"/>
       <c r="E25" s="17" t="s">
         <v>16</v>
@@ -1178,16 +1185,6 @@
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="I3:J3"/>
-    <mergeCell ref="I4:J4"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E4:F4"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
@@ -1202,6 +1199,16 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="C8:C11"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="I3:J3"/>
+    <mergeCell ref="I4:J4"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>